<commit_message>
[UPDATE] Delete first row data for using excel data
</commit_message>
<xml_diff>
--- a/RPG_Game/PlaceData.xlsx
+++ b/RPG_Game/PlaceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TeamSparta\PersonalProject\RPG_Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896C050F-6A30-4265-9508-203499B0B026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0519AC3D-0414-4E20-A694-A803865CEFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11565" yWindow="3135" windowWidth="16020" windowHeight="12465" xr2:uid="{288195C0-BF66-4B03-812C-610F85EA7E9A}"/>
+    <workbookView xWindow="5595" yWindow="3135" windowWidth="16020" windowHeight="12465" xr2:uid="{288195C0-BF66-4B03-812C-610F85EA7E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,9 +458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916C3D32-73B2-4E29-A1B0-939B6863675E}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -526,6 +528,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1004</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[UPDATE] clear Assignment2, Added class Character and CharacterData make ModifiedDisplay
</commit_message>
<xml_diff>
--- a/RPG_Game/PlaceData.xlsx
+++ b/RPG_Game/PlaceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TeamSparta\PersonalProject\RPG_Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF0D5DE-1425-4FC4-ABF0-8AEFDA4C91D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648575F2-F26F-4883-A8E3-4260E024F125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="3135" windowWidth="16020" windowHeight="12465" xr2:uid="{288195C0-BF66-4B03-812C-610F85EA7E9A}"/>
+    <workbookView xWindow="10890" yWindow="3135" windowWidth="16020" windowHeight="12465" xr2:uid="{288195C0-BF66-4B03-812C-610F85EA7E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,10 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{1001,1002}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>다람쥐가 나오는 사냥터</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -226,6 +222,22 @@
   </si>
   <si>
     <t>{1001,1003,1004,1005}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>능력치보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{1003}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{10001,1001,1002}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -596,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916C3D32-73B2-4E29-A1B0-939B6863675E}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -629,13 +641,13 @@
         <v>1001</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -649,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -663,7 +675,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -671,13 +683,13 @@
         <v>1021</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -685,13 +697,13 @@
         <v>1022</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -699,13 +711,13 @@
         <v>1023</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -713,13 +725,13 @@
         <v>1024</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -727,13 +739,13 @@
         <v>1025</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -741,13 +753,13 @@
         <v>1031</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -755,13 +767,13 @@
         <v>1032</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -769,13 +781,13 @@
         <v>1033</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -783,13 +795,13 @@
         <v>1034</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -797,13 +809,13 @@
         <v>1035</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
         <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -811,13 +823,13 @@
         <v>1004</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
         <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -825,13 +837,27 @@
         <v>1005</v>
       </c>
       <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>10001</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPDATE] Add '\n' with different type of Selection
</commit_message>
<xml_diff>
--- a/RPG_Game/PlaceData.xlsx
+++ b/RPG_Game/PlaceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TeamSparta\PersonalProject\RPG_Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648575F2-F26F-4883-A8E3-4260E024F125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6132896B-C610-49FC-BF14-33B1D6CB9806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10890" yWindow="3135" windowWidth="16020" windowHeight="12465" xr2:uid="{288195C0-BF66-4B03-812C-610F85EA7E9A}"/>
   </bookViews>
@@ -46,14 +46,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Selections</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PlaceID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>마을 번화가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -238,6 +230,16 @@
   </si>
   <si>
     <t>{10001,1001,1002}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Selections ( 빈칸없이 )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlaceID
+일반맵 &lt;10000
+특별맵 &gt;10000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -284,7 +286,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -293,6 +295,12 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,29 +619,30 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="17.375" customWidth="1"/>
     <col min="3" max="3" width="31.125" customWidth="1"/>
     <col min="4" max="4" width="29.75" customWidth="1"/>
     <col min="5" max="5" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="D1" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -641,13 +650,13 @@
         <v>1001</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -655,13 +664,13 @@
         <v>1002</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -669,13 +678,13 @@
         <v>1003</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -683,13 +692,13 @@
         <v>1021</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -697,13 +706,13 @@
         <v>1022</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -711,13 +720,13 @@
         <v>1023</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -725,13 +734,13 @@
         <v>1024</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -739,13 +748,13 @@
         <v>1025</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -753,13 +762,13 @@
         <v>1031</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -767,13 +776,13 @@
         <v>1032</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -781,13 +790,13 @@
         <v>1033</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -795,13 +804,13 @@
         <v>1034</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -809,13 +818,13 @@
         <v>1035</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -823,13 +832,13 @@
         <v>1004</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -837,13 +846,13 @@
         <v>1005</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
         <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -851,13 +860,13 @@
         <v>10001</v>
       </c>
       <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" t="s">
-        <v>49</v>
-      </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPDATE] Add ItemData excel sheet
</commit_message>
<xml_diff>
--- a/RPG_Game/PlaceData.xlsx
+++ b/RPG_Game/PlaceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TeamSparta\PersonalProject\RPG_Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6132896B-C610-49FC-BF14-33B1D6CB9806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5019EAAC-9027-431A-ADDA-C8B6D85D7B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10890" yWindow="3135" windowWidth="16020" windowHeight="12465" xr2:uid="{288195C0-BF66-4B03-812C-610F85EA7E9A}"/>
   </bookViews>
@@ -42,10 +42,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>마을 번화가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -222,10 +218,6 @@
   </si>
   <si>
     <t>{1003}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -240,6 +232,15 @@
     <t>PlaceID
 일반맵 &lt;10000
 특별맵 &gt;10000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description 
+(설명이 없으면 빈칸하나 입력)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -619,7 +620,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -633,16 +634,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -650,13 +651,13 @@
         <v>1001</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -664,13 +665,13 @@
         <v>1002</v>
       </c>
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -678,13 +679,13 @@
         <v>1003</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,13 +693,13 @@
         <v>1021</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -706,13 +707,13 @@
         <v>1022</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -720,13 +721,13 @@
         <v>1023</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -734,13 +735,13 @@
         <v>1024</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -748,13 +749,13 @@
         <v>1025</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
         <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -762,13 +763,13 @@
         <v>1031</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -776,13 +777,13 @@
         <v>1032</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -790,13 +791,13 @@
         <v>1033</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -804,13 +805,13 @@
         <v>1034</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -818,13 +819,13 @@
         <v>1035</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -832,13 +833,13 @@
         <v>1004</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
         <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="33" x14ac:dyDescent="0.3">
@@ -846,13 +847,13 @@
         <v>1005</v>
       </c>
       <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -860,13 +861,13 @@
         <v>10001</v>
       </c>
       <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>